<commit_message>
clread build and updatedreadme
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel Files/TestData.xlsx
+++ b/src/test/resources/Excel Files/TestData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D40AAE-3D9A-46E7-A3E2-764ECCA8B8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE79B2F4-A649-4CE7-A152-990F18CC4CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8976" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FileData" sheetId="8" r:id="rId1"/>
-    <sheet name="EditData" sheetId="5" r:id="rId2"/>
+    <sheet name="SignUpTest" sheetId="8" r:id="rId1"/>
+    <sheet name="SearchItem" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>

</xml_diff>